<commit_message>
update strategy configuration files on jinrui servers
</commit_message>
<xml_diff>
--- a/ExplorerFund/operation/checklist/运维事项确认表.xlsx
+++ b/ExplorerFund/operation/checklist/运维事项确认表.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -87,14 +87,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>上期</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>日盘</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>郑州</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -103,17 +95,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">今天郑州夜盘测试zzta 1 手，需要配置ev文件，待会儿教授传上来
+    <t>passed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">其中
+(ok) fl34_cf_night, (ok)fl34_ta_night各给3手； 
+(OK) fl50的各给1手
+，fl50的策略需要配置文件
 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">(ok) 明天日盘ru先做1手，fl34_ru_day.so
-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>passed</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -254,8 +244,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A2:F16" totalsRowShown="0">
-  <autoFilter ref="A2:F16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A2:F15" totalsRowShown="0">
+  <autoFilter ref="A2:F15">
     <filterColumn colId="2"/>
     <filterColumn colId="4"/>
     <filterColumn colId="5"/>
@@ -557,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -596,7 +586,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="40.5" customHeight="1">
+    <row r="3" spans="1:6" ht="104.25" customHeight="1">
       <c r="B3" s="6" t="s">
         <v>10</v>
       </c>
@@ -606,51 +596,34 @@
       <c r="D3" s="7">
         <v>42731</v>
       </c>
-      <c r="E3" s="11" t="s">
-        <v>16</v>
+      <c r="E3" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="55.5" customHeight="1">
       <c r="B4" s="6" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D4" s="7">
-        <v>42731</v>
+        <v>42745</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>14</v>
+        <v>8</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="55.5" customHeight="1">
-      <c r="B5" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="7">
-        <v>42745</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="7"/>
+    <row r="5" spans="1:6">
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>